<commit_message>
-added startup time (delay) constraint for gas turbine -updated some example case parameters
</commit_message>
<xml_diff>
--- a/data_example2.xlsx
+++ b/data_example2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5A1840-FAA3-4DA2-BF3A-89A6DC14AA95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34B2199-15BD-4AB0-966C-47AA0AD7097D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11508" yWindow="276" windowWidth="15336" windowHeight="16356" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="4836" yWindow="1152" windowWidth="17280" windowHeight="10872" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="168">
   <si>
     <t>id</t>
   </si>
@@ -395,9 +395,6 @@
     <t>co2_tax</t>
   </si>
   <si>
-    <t>$/kgCO2</t>
-  </si>
-  <si>
     <t>seawater inlet</t>
   </si>
   <si>
@@ -524,7 +521,28 @@
     <t>forecast_timesteps</t>
   </si>
   <si>
-    <t>number of timesteps in planning horizon (6 hours)</t>
+    <t>1/60 = full power in 60 minutes</t>
+  </si>
+  <si>
+    <t>wells</t>
+  </si>
+  <si>
+    <t>water wells</t>
+  </si>
+  <si>
+    <t>startupDelay</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>number of timesteps in planning horizon</t>
+  </si>
+  <si>
+    <t>slightly more than gt1 to give preference to gt1</t>
+  </si>
+  <si>
+    <t>$/kgCO2 (40 eur per tonne)</t>
   </si>
 </sst>
 </file>
@@ -895,7 +913,7 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,7 +1012,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1196,10 +1214,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00A70904-C380-433D-9493-9658C938F213}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,7 +1469,7 @@
         <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -1474,13 +1492,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1489,7 +1507,7 @@
         <v>10000</v>
       </c>
       <c r="H11">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="I11">
         <v>100</v>
@@ -1500,13 +1518,13 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -1518,7 +1536,7 @@
         <v>0.01</v>
       </c>
       <c r="I12">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="J12">
         <v>300</v>
@@ -1526,13 +1544,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>80</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1544,7 +1562,7 @@
         <v>0.01</v>
       </c>
       <c r="I13">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J13">
         <v>300</v>
@@ -1552,13 +1570,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1578,13 +1596,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1596,7 +1614,7 @@
         <v>0.01</v>
       </c>
       <c r="I15">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="J15">
         <v>300</v>
@@ -1607,10 +1625,10 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1622,7 +1640,7 @@
         <v>0.01</v>
       </c>
       <c r="I16">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="J16">
         <v>300</v>
@@ -1630,13 +1648,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1645,7 +1663,7 @@
         <v>10000</v>
       </c>
       <c r="H17">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="I17">
         <v>100</v>
@@ -1656,10 +1674,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C18" t="s">
         <v>59</v>
@@ -1674,7 +1692,7 @@
         <v>0.1</v>
       </c>
       <c r="I18">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="J18">
         <v>300</v>
@@ -1682,47 +1700,73 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="H19">
-        <v>0.01</v>
+        <v>0.1</v>
+      </c>
+      <c r="I19">
+        <v>200</v>
+      </c>
+      <c r="J19">
+        <v>300</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1000</v>
+      </c>
+      <c r="H20">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>81</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
         <v>500</v>
       </c>
-      <c r="F20">
+      <c r="F21">
         <v>1E-3</v>
       </c>
-      <c r="G20">
+      <c r="G21">
         <v>0.01</v>
       </c>
-      <c r="H20">
+      <c r="H21">
         <v>0.01</v>
       </c>
     </row>
@@ -2223,7 +2267,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E19">
         <v>15</v>
@@ -2370,7 +2414,7 @@
         <v>80</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -2382,7 +2426,7 @@
         <v>0</v>
       </c>
       <c r="G25" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="P25">
         <v>0.7</v>
@@ -2395,10 +2439,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB366907-93DA-4245-BEBF-19818450F8D2}">
-  <dimension ref="A1:J46"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2436,10 +2480,10 @@
         <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
@@ -2476,7 +2520,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2491,7 +2535,7 @@
         <v>37</v>
       </c>
       <c r="F3">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -2500,7 +2544,7 @@
         <v>40</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2508,7 +2552,7 @@
         <v>41</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2527,6 +2571,9 @@
         <f>1/60</f>
         <v>1.6666666666666666E-2</v>
       </c>
+      <c r="J6" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H7" t="s">
@@ -2538,62 +2585,67 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="H8" t="s">
+        <v>163</v>
+      </c>
+      <c r="I8">
+        <v>15</v>
+      </c>
+      <c r="J8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
         <v>88</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>65</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>37</v>
       </c>
-      <c r="F8">
-        <v>15</v>
-      </c>
-      <c r="G8">
+      <c r="F9">
+        <v>25</v>
+      </c>
+      <c r="G9">
         <v>0</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H9" t="s">
         <v>40</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H9" t="s">
-        <v>41</v>
-      </c>
       <c r="I9">
-        <v>1</v>
+        <v>2.36</v>
+      </c>
+      <c r="J9" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="I10">
-        <v>0.05</v>
+        <v>0.53</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H11" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="I11">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I12">
         <f>1/60</f>
@@ -2601,326 +2653,300 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13">
-        <v>1000</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
       <c r="H13" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="I13">
-        <v>0.4</v>
-      </c>
-      <c r="J13" t="s">
-        <v>148</v>
+        <f>1/60</f>
+        <v>1.6666666666666666E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H14" t="s">
+        <v>163</v>
+      </c>
+      <c r="I14">
+        <v>15</v>
+      </c>
+      <c r="J14" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15">
+        <v>1000</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I15">
+        <v>0.4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>145</v>
+      </c>
+      <c r="I16">
+        <v>300</v>
+      </c>
+      <c r="J16" t="s">
         <v>146</v>
       </c>
-      <c r="I14">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H17" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I17">
+        <v>20</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>1000</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18">
+        <v>0.2</v>
+      </c>
+      <c r="J18" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>145</v>
+      </c>
+      <c r="I19">
         <v>300</v>
       </c>
-      <c r="J14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H15" s="2" t="s">
+      <c r="J19" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H20" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="I20">
+        <v>20</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="I15">
-        <v>20</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16">
-        <v>1000</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16">
-        <v>0.2</v>
-      </c>
-      <c r="J16" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H17" t="s">
-        <v>146</v>
-      </c>
-      <c r="I17">
-        <v>300</v>
-      </c>
-      <c r="J17" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H18" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="I18">
-        <v>20</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19">
-        <v>1000</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>39</v>
-      </c>
-      <c r="I19">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H20" t="s">
-        <v>110</v>
-      </c>
-      <c r="I20">
-        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21">
+        <v>1000</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H22" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
         <v>128</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" t="s">
-        <v>129</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="E23" t="s">
         <v>36</v>
       </c>
-      <c r="F21">
+      <c r="F23">
         <v>5</v>
       </c>
-      <c r="G21">
+      <c r="G23">
         <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
-      <c r="D22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E22" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22">
-        <v>20</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
-        <v>158</v>
-      </c>
-      <c r="I22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H23" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D24" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I24">
-        <v>3</v>
+        <v>157</v>
+      </c>
+      <c r="I24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
-      </c>
-      <c r="G25">
-        <v>3</v>
+      <c r="H25" t="s">
+        <v>58</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>45</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F26">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
+      <c r="H26" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="D27" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="F27">
-        <v>1000</v>
+        <v>5</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>15</v>
       </c>
       <c r="E28" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="F28">
         <v>1000</v>
@@ -2931,19 +2957,19 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="s">
         <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="F29">
         <v>1000</v>
@@ -2954,19 +2980,19 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="E30" t="s">
-        <v>57</v>
+        <v>92</v>
       </c>
       <c r="F30">
         <v>1000</v>
@@ -2974,132 +3000,138 @@
       <c r="G30">
         <v>0</v>
       </c>
-      <c r="H30" t="s">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31">
+        <v>1000</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>130</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32">
+        <v>1000</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
         <v>58</v>
       </c>
-      <c r="I30">
+      <c r="I32">
         <f>270/0.1</f>
         <v>2700</v>
       </c>
-      <c r="J30" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>138</v>
-      </c>
-      <c r="B31">
+      <c r="J32" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33">
         <v>0</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>88</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>14</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E33" t="s">
         <v>42</v>
       </c>
-      <c r="F31">
+      <c r="F33">
         <v>4</v>
       </c>
-      <c r="G31">
+      <c r="G33">
         <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" t="s">
-        <v>69</v>
-      </c>
-      <c r="E32" t="s">
-        <v>70</v>
-      </c>
-      <c r="F32">
-        <v>4</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32" t="s">
-        <v>39</v>
-      </c>
-      <c r="I32">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H33" t="s">
-        <v>71</v>
-      </c>
-      <c r="I33">
-        <v>2</v>
-      </c>
-      <c r="J33" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F34">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="I34">
-        <v>6</v>
-      </c>
-      <c r="J34" t="s">
-        <v>144</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H35" t="s">
-        <v>158</v>
-      </c>
-      <c r="I35" t="s">
-        <v>56</v>
+        <v>71</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="J35" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="D36" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E36" t="s">
         <v>76</v>
@@ -3122,7 +3154,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I37" t="s">
         <v>56</v>
@@ -3130,16 +3162,16 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>72</v>
+        <v>161</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E38" t="s">
         <v>76</v>
@@ -3157,12 +3189,12 @@
         <v>6</v>
       </c>
       <c r="J38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I39" t="s">
         <v>56</v>
@@ -3170,57 +3202,42 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>161</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F40">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
+      <c r="H40" t="s">
+        <v>50</v>
+      </c>
+      <c r="I40">
+        <v>6</v>
+      </c>
+      <c r="J40" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>139</v>
-      </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" t="s">
-        <v>97</v>
-      </c>
-      <c r="E41" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41">
-        <v>1000</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
       <c r="H41" t="s">
-        <v>39</v>
-      </c>
-      <c r="I41">
-        <v>0.8</v>
-      </c>
-      <c r="J41" t="s">
-        <v>151</v>
+        <v>157</v>
+      </c>
+      <c r="I41" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
@@ -3228,93 +3245,148 @@
         <v>140</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" t="s">
         <v>80</v>
       </c>
       <c r="D42" t="s">
+        <v>93</v>
+      </c>
+      <c r="E42" t="s">
+        <v>94</v>
+      </c>
+      <c r="F42">
+        <v>1000</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>138</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" t="s">
+        <v>97</v>
+      </c>
+      <c r="E43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43">
+        <v>1000</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43" t="s">
+        <v>39</v>
+      </c>
+      <c r="I43">
+        <v>0.8</v>
+      </c>
+      <c r="J43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" t="s">
         <v>98</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E44" t="s">
         <v>99</v>
       </c>
-      <c r="F42">
-        <v>0.13</v>
-      </c>
-      <c r="G42">
-        <v>0.13</v>
-      </c>
-      <c r="H42" t="s">
+      <c r="F44">
+        <v>1.3</v>
+      </c>
+      <c r="G44">
+        <v>1.3</v>
+      </c>
+      <c r="H44" t="s">
         <v>39</v>
       </c>
-      <c r="I42">
+      <c r="I44">
         <v>0.8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H43" t="s">
-        <v>152</v>
-      </c>
-      <c r="I43">
-        <v>6</v>
-      </c>
-      <c r="J43" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H44" t="s">
-        <v>155</v>
-      </c>
-      <c r="I44">
-        <v>0.13</v>
-      </c>
-      <c r="J44" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H45" t="s">
+        <v>151</v>
+      </c>
+      <c r="I45">
+        <v>6</v>
+      </c>
+      <c r="J45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H46" t="s">
+        <v>154</v>
+      </c>
+      <c r="I46">
+        <v>1.3</v>
+      </c>
+      <c r="J46" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H47" t="s">
         <v>71</v>
       </c>
-      <c r="I45">
-        <v>0.13</v>
-      </c>
-      <c r="J45" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>133</v>
-      </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" t="s">
-        <v>80</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="I47">
+        <v>1.3</v>
+      </c>
+      <c r="J47" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>161</v>
+      </c>
+      <c r="D48" t="s">
+        <v>162</v>
+      </c>
+      <c r="E48" t="s">
         <v>119</v>
       </c>
-      <c r="E46" t="s">
-        <v>120</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46">
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48">
         <v>0</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H48" t="s">
         <v>50</v>
       </c>
-      <c r="I46">
+      <c r="I48">
         <v>0.7</v>
       </c>
-      <c r="J46" t="s">
-        <v>143</v>
+      <c r="J48" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3328,7 +3400,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3365,10 +3437,10 @@
         <v>53</v>
       </c>
       <c r="B3">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3384,13 +3456,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B5">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -3398,10 +3470,10 @@
         <v>117</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -9884,21 +9956,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -10107,24 +10164,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10141,4 +10196,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
per second instead of per hour
</commit_message>
<xml_diff>
--- a/data_example2.xlsx
+++ b/data_example2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hsven\code\hybrid_energy_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34B2199-15BD-4AB0-966C-47AA0AD7097D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A96964-CC16-4BB9-87F0-F7F434641A18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4836" yWindow="1152" windowWidth="17280" windowHeight="10872" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="11076" activeTab="3" xr2:uid="{67DC4D86-39E4-4DA3-B21D-C0F42277600B}"/>
   </bookViews>
   <sheets>
     <sheet name="node" sheetId="1" r:id="rId1"/>
@@ -521,9 +521,6 @@
     <t>forecast_timesteps</t>
   </si>
   <si>
-    <t>1/60 = full power in 60 minutes</t>
-  </si>
-  <si>
     <t>wells</t>
   </si>
   <si>
@@ -543,6 +540,9 @@
   </si>
   <si>
     <t>$/kgCO2 (40 eur per tonne)</t>
+  </si>
+  <si>
+    <t>0.5=50% of ull load per minute</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1469,7 +1469,7 @@
         <v>101</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -1495,7 +1495,7 @@
         <v>78</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C11" t="s">
         <v>80</v>
@@ -2442,7 +2442,7 @@
   <dimension ref="A1:J48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2538,7 +2538,7 @@
         <v>25</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
         <v>40</v>
@@ -2568,11 +2568,10 @@
         <v>67</v>
       </c>
       <c r="I6">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
+        <v>0.5</v>
       </c>
       <c r="J6" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2580,19 +2579,18 @@
         <v>68</v>
       </c>
       <c r="I7">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
         <v>163</v>
-      </c>
-      <c r="I8">
-        <v>15</v>
-      </c>
-      <c r="J8" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2615,7 +2613,7 @@
         <v>25</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H9" t="s">
         <v>40</v>
@@ -2624,7 +2622,7 @@
         <v>2.36</v>
       </c>
       <c r="J9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2648,8 +2646,7 @@
         <v>67</v>
       </c>
       <c r="I12">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -2657,19 +2654,18 @@
         <v>68</v>
       </c>
       <c r="I13">
-        <f>1/60</f>
-        <v>1.6666666666666666E-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H14" t="s">
+        <v>162</v>
+      </c>
+      <c r="I14">
+        <v>10</v>
+      </c>
+      <c r="J14" t="s">
         <v>163</v>
-      </c>
-      <c r="I14">
-        <v>15</v>
-      </c>
-      <c r="J14" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -3128,7 +3124,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D36" t="s">
         <v>73</v>
@@ -3168,7 +3164,7 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D38" t="s">
         <v>74</v>
@@ -3208,7 +3204,7 @@
         <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D40" t="s">
         <v>75</v>
@@ -3365,10 +3361,10 @@
         <v>1</v>
       </c>
       <c r="C48" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" t="s">
         <v>161</v>
-      </c>
-      <c r="D48" t="s">
-        <v>162</v>
       </c>
       <c r="E48" t="s">
         <v>119</v>
@@ -3440,7 +3436,7 @@
         <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3473,7 +3469,7 @@
         <v>0.04</v>
       </c>
       <c r="C6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -9956,6 +9952,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010068757AD89D0841429F5831BBC6267AC1" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e521892cf07d8fee7d1fab9fe3aaa83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c" xmlns:ns4="53f6e7f0-9e34-4545-9b50-e54ccadfb78a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ffc55c83d6521c05fad87c69f289641" ns3:_="" ns4:_="">
     <xsd:import namespace="78e0c6f3-9112-4e2d-9710-8a99a0c0b95c"/>
@@ -10164,22 +10175,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1016DCAE-9D9F-40DE-A38A-1587953D2A7E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10196,21 +10209,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B20FA7CB-4913-4ED5-B2A6-1FAA15DCEB4D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78762D46-3C96-44E4-BFC9-B88DF736E950}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>